<commit_message>
Instanciamento dos dados de tipo de registro
</commit_message>
<xml_diff>
--- a/dados/estabelecimentos/ago17.xlsx
+++ b/dados/estabelecimentos/ago17.xlsx
@@ -14,9 +14,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83">
-  <si>
-    <t>CNES - Estabelecimentos por Tipo - Paraná</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82">
+  <si>
+    <t>CNES 0 Estabelecimentos por Tipo 0 Paraná</t>
   </si>
   <si>
     <t>Quantidade por Tipo de Estabelecimento e Tipo de Gestão</t>
@@ -46,9 +46,6 @@
     <t>CENTRAL DE REGUALAÇÃO</t>
   </si>
   <si>
-    <t>-</t>
-  </si>
-  <si>
     <t>Centro de Regulação de Serviços de Saúde</t>
   </si>
   <si>
@@ -73,7 +70,7 @@
     <t>CntrAtcHem</t>
   </si>
   <si>
-    <t>CENTRO DE ATENÇÃO PSICOSSOCIAL-CAPS</t>
+    <t>CENTRO DE ATENÇÃO PSICOSSOCIAL0CAPS</t>
   </si>
   <si>
     <t>Centro de Atenção Psicossocial</t>
@@ -181,7 +178,7 @@
     <t>SadtIso</t>
   </si>
   <si>
-    <t>UNIDADE MOVEL DE NIVEL PRE-HOSP-URGENCIA/EMERGENCI</t>
+    <t>UNIDADE MOVEL DE NIVEL PRE0HOSP0URGENCIA/EMERGENCI</t>
   </si>
   <si>
     <t>Unidade Móvel de Nível Pré0Hospitalar na área de Urgência Samu</t>
@@ -217,7 +214,7 @@
     <t>CnrtTransp</t>
   </si>
   <si>
-    <t xml:space="preserve"> Fonte: Ministério da Saúde - Cadastro Nacional dos Estabelecimentos de Saúde do Brasil - CNES</t>
+    <t xml:space="preserve"> Fonte: Ministério da Saúde 0 Cadastro Nacional dos Estabelecimentos de Saúde do Brasil 0 CNES</t>
   </si>
   <si>
     <t xml:space="preserve"> Nota:</t>
@@ -271,9 +268,9 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
     <numFmt numFmtId="176" formatCode="_-&quot;R$&quot;* #,##0.00_-;\-&quot;R$&quot;* #,##0.00_-;_-&quot;R$&quot;* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="177" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="177" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="178" formatCode="_-&quot;R$&quot;* #,##0_-;\-&quot;R$&quot;* #,##0_-;_-&quot;R$&quot;* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="179" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="179" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="20">
     <font>
@@ -284,6 +281,44 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -300,14 +335,6 @@
     </font>
     <font>
       <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
       <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
@@ -315,9 +342,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
       <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -331,14 +357,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -346,7 +365,14 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -368,8 +394,17 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -383,46 +418,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -437,37 +434,175 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -479,145 +614,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -628,6 +625,17 @@
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -655,26 +663,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FF7F7F7F"/>
       </left>
@@ -693,8 +681,8 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -728,153 +716,162 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="13" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="20" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="16" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="27" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="27" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="16" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="24" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="13" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="13" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1203,8 +1200,8 @@
   <sheetPr/>
   <dimension ref="A1:H55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11:E11"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.2857142857143" defaultRowHeight="12.75" outlineLevelCol="7"/>
@@ -1254,8 +1251,8 @@
       <c r="A6" t="s">
         <v>9</v>
       </c>
-      <c r="B6" t="s">
-        <v>10</v>
+      <c r="B6">
+        <v>0</v>
       </c>
       <c r="C6">
         <v>1</v>
@@ -1267,67 +1264,67 @@
         <v>2</v>
       </c>
       <c r="G6" t="s">
+        <v>10</v>
+      </c>
+      <c r="H6" t="s">
         <v>11</v>
-      </c>
-      <c r="H6" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="7" spans="1:8">
       <c r="A7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7">
+        <v>0</v>
+      </c>
+      <c r="C7">
+        <v>0</v>
+      </c>
+      <c r="D7">
+        <v>1</v>
+      </c>
+      <c r="E7">
+        <v>1</v>
+      </c>
+      <c r="G7" t="s">
         <v>13</v>
       </c>
-      <c r="B7" t="s">
-        <v>10</v>
-      </c>
-      <c r="C7" t="s">
-        <v>10</v>
-      </c>
-      <c r="D7">
-        <v>1</v>
-      </c>
-      <c r="E7">
-        <v>1</v>
-      </c>
-      <c r="G7" t="s">
+      <c r="H7" t="s">
         <v>14</v>
-      </c>
-      <c r="H7" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="8" spans="1:8">
       <c r="A8" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8">
+        <v>0</v>
+      </c>
+      <c r="C8">
+        <v>1</v>
+      </c>
+      <c r="D8">
+        <v>0</v>
+      </c>
+      <c r="E8">
+        <v>1</v>
+      </c>
+      <c r="G8" t="s">
         <v>16</v>
       </c>
-      <c r="B8" t="s">
-        <v>10</v>
-      </c>
-      <c r="C8">
-        <v>1</v>
-      </c>
-      <c r="D8" t="s">
-        <v>10</v>
-      </c>
-      <c r="E8">
-        <v>1</v>
-      </c>
-      <c r="G8" t="s">
+      <c r="H8" t="s">
         <v>17</v>
-      </c>
-      <c r="H8" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="9" spans="1:8">
       <c r="A9" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B9">
         <v>1</v>
       </c>
-      <c r="C9" t="s">
-        <v>10</v>
+      <c r="C9">
+        <v>0</v>
       </c>
       <c r="D9">
         <v>12</v>
@@ -1336,21 +1333,21 @@
         <v>13</v>
       </c>
       <c r="G9" t="s">
+        <v>19</v>
+      </c>
+      <c r="H9" t="s">
         <v>20</v>
-      </c>
-      <c r="H9" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="10" spans="1:8">
       <c r="A10" t="s">
-        <v>22</v>
-      </c>
-      <c r="B10" t="s">
-        <v>10</v>
-      </c>
-      <c r="C10" t="s">
-        <v>10</v>
+        <v>21</v>
+      </c>
+      <c r="B10">
+        <v>0</v>
+      </c>
+      <c r="C10">
+        <v>0</v>
       </c>
       <c r="D10">
         <v>111</v>
@@ -1359,38 +1356,38 @@
         <v>111</v>
       </c>
       <c r="G10" t="s">
+        <v>22</v>
+      </c>
+      <c r="H10" t="s">
         <v>23</v>
-      </c>
-      <c r="H10" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="11" spans="1:8">
       <c r="A11" t="s">
+        <v>24</v>
+      </c>
+      <c r="B11">
+        <v>0</v>
+      </c>
+      <c r="C11">
+        <v>0</v>
+      </c>
+      <c r="D11">
+        <v>1</v>
+      </c>
+      <c r="E11">
+        <v>1</v>
+      </c>
+      <c r="G11" t="s">
         <v>25</v>
       </c>
-      <c r="B11" t="s">
-        <v>10</v>
-      </c>
-      <c r="C11" t="s">
-        <v>10</v>
-      </c>
-      <c r="D11">
-        <v>1</v>
-      </c>
-      <c r="E11">
-        <v>1</v>
-      </c>
-      <c r="G11" t="s">
+      <c r="H11" t="s">
         <v>26</v>
-      </c>
-      <c r="H11" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="12" spans="1:8">
       <c r="A12" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B12">
         <v>2</v>
@@ -1405,21 +1402,21 @@
         <v>365</v>
       </c>
       <c r="G12" t="s">
+        <v>28</v>
+      </c>
+      <c r="H12" t="s">
         <v>29</v>
-      </c>
-      <c r="H12" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="13" spans="1:8">
       <c r="A13" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B13">
         <v>2</v>
       </c>
-      <c r="C13" t="s">
-        <v>10</v>
+      <c r="C13">
+        <v>0</v>
       </c>
       <c r="D13">
         <v>16</v>
@@ -1428,15 +1425,15 @@
         <v>18</v>
       </c>
       <c r="G13" t="s">
+        <v>31</v>
+      </c>
+      <c r="H13" t="s">
         <v>32</v>
-      </c>
-      <c r="H13" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="14" spans="1:8">
       <c r="A14" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B14">
         <v>6</v>
@@ -1451,44 +1448,44 @@
         <v>42</v>
       </c>
       <c r="G14" t="s">
+        <v>34</v>
+      </c>
+      <c r="H14" t="s">
         <v>35</v>
-      </c>
-      <c r="H14" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="15" spans="1:8">
       <c r="A15" t="s">
+        <v>36</v>
+      </c>
+      <c r="B15">
+        <v>0</v>
+      </c>
+      <c r="C15">
+        <v>1</v>
+      </c>
+      <c r="D15">
+        <v>0</v>
+      </c>
+      <c r="E15">
+        <v>1</v>
+      </c>
+      <c r="G15" t="s">
         <v>37</v>
       </c>
-      <c r="B15" t="s">
-        <v>10</v>
-      </c>
-      <c r="C15">
-        <v>1</v>
-      </c>
-      <c r="D15" t="s">
-        <v>10</v>
-      </c>
-      <c r="E15">
-        <v>1</v>
-      </c>
-      <c r="G15" t="s">
+      <c r="H15" t="s">
         <v>38</v>
-      </c>
-      <c r="H15" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="16" spans="1:8">
       <c r="A16" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B16">
         <v>3</v>
       </c>
-      <c r="C16" t="s">
-        <v>10</v>
+      <c r="C16">
+        <v>0</v>
       </c>
       <c r="D16">
         <v>407</v>
@@ -1497,21 +1494,21 @@
         <v>410</v>
       </c>
       <c r="G16" t="s">
+        <v>40</v>
+      </c>
+      <c r="H16" t="s">
         <v>41</v>
-      </c>
-      <c r="H16" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="17" spans="1:8">
       <c r="A17" t="s">
-        <v>43</v>
-      </c>
-      <c r="B17" t="s">
-        <v>10</v>
-      </c>
-      <c r="C17" t="s">
-        <v>10</v>
+        <v>42</v>
+      </c>
+      <c r="B17">
+        <v>0</v>
+      </c>
+      <c r="C17">
+        <v>0</v>
       </c>
       <c r="D17">
         <v>9</v>
@@ -1520,18 +1517,18 @@
         <v>9</v>
       </c>
       <c r="G17" t="s">
+        <v>43</v>
+      </c>
+      <c r="H17" t="s">
         <v>44</v>
-      </c>
-      <c r="H17" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="18" spans="1:8">
       <c r="A18" t="s">
-        <v>46</v>
-      </c>
-      <c r="B18" t="s">
-        <v>10</v>
+        <v>45</v>
+      </c>
+      <c r="B18">
+        <v>0</v>
       </c>
       <c r="C18">
         <v>2</v>
@@ -1543,21 +1540,21 @@
         <v>14</v>
       </c>
       <c r="G18" t="s">
+        <v>46</v>
+      </c>
+      <c r="H18" t="s">
         <v>47</v>
-      </c>
-      <c r="H18" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="19" spans="1:8">
       <c r="A19" t="s">
-        <v>49</v>
-      </c>
-      <c r="B19" t="s">
-        <v>10</v>
-      </c>
-      <c r="C19" t="s">
-        <v>10</v>
+        <v>48</v>
+      </c>
+      <c r="B19">
+        <v>0</v>
+      </c>
+      <c r="C19">
+        <v>0</v>
       </c>
       <c r="D19">
         <v>19</v>
@@ -1566,15 +1563,15 @@
         <v>19</v>
       </c>
       <c r="G19" t="s">
+        <v>49</v>
+      </c>
+      <c r="H19" t="s">
         <v>50</v>
-      </c>
-      <c r="H19" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="20" spans="1:8">
       <c r="A20" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B20">
         <v>16</v>
@@ -1589,21 +1586,21 @@
         <v>483</v>
       </c>
       <c r="G20" t="s">
+        <v>52</v>
+      </c>
+      <c r="H20" t="s">
         <v>53</v>
-      </c>
-      <c r="H20" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="21" spans="1:8">
       <c r="A21" t="s">
-        <v>55</v>
-      </c>
-      <c r="B21" t="s">
-        <v>10</v>
-      </c>
-      <c r="C21" t="s">
-        <v>10</v>
+        <v>54</v>
+      </c>
+      <c r="B21">
+        <v>0</v>
+      </c>
+      <c r="C21">
+        <v>0</v>
       </c>
       <c r="D21">
         <v>29</v>
@@ -1612,79 +1609,79 @@
         <v>29</v>
       </c>
       <c r="G21" t="s">
+        <v>55</v>
+      </c>
+      <c r="H21" t="s">
         <v>56</v>
-      </c>
-      <c r="H21" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="22" spans="1:8">
       <c r="A22" t="s">
+        <v>57</v>
+      </c>
+      <c r="B22">
+        <v>1</v>
+      </c>
+      <c r="C22">
+        <v>0</v>
+      </c>
+      <c r="D22">
+        <v>0</v>
+      </c>
+      <c r="E22">
+        <v>1</v>
+      </c>
+      <c r="G22" t="s">
         <v>58</v>
       </c>
-      <c r="B22">
-        <v>1</v>
-      </c>
-      <c r="C22" t="s">
-        <v>10</v>
-      </c>
-      <c r="D22" t="s">
-        <v>10</v>
-      </c>
-      <c r="E22">
-        <v>1</v>
-      </c>
-      <c r="G22" t="s">
+      <c r="H22" t="s">
         <v>59</v>
-      </c>
-      <c r="H22" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="23" spans="1:8">
       <c r="A23" t="s">
+        <v>60</v>
+      </c>
+      <c r="B23">
+        <v>0</v>
+      </c>
+      <c r="C23">
+        <v>0</v>
+      </c>
+      <c r="D23">
+        <v>1</v>
+      </c>
+      <c r="E23">
+        <v>1</v>
+      </c>
+      <c r="G23" t="s">
         <v>61</v>
       </c>
-      <c r="B23" t="s">
-        <v>10</v>
-      </c>
-      <c r="C23" t="s">
-        <v>10</v>
-      </c>
-      <c r="D23">
-        <v>1</v>
-      </c>
-      <c r="E23">
-        <v>1</v>
-      </c>
-      <c r="G23" t="s">
+      <c r="H23" t="s">
         <v>62</v>
-      </c>
-      <c r="H23" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="24" spans="1:8">
       <c r="A24" t="s">
+        <v>63</v>
+      </c>
+      <c r="B24">
+        <v>0</v>
+      </c>
+      <c r="C24">
+        <v>1</v>
+      </c>
+      <c r="D24">
+        <v>0</v>
+      </c>
+      <c r="E24">
+        <v>1</v>
+      </c>
+      <c r="G24" t="s">
         <v>64</v>
       </c>
-      <c r="B24" t="s">
-        <v>10</v>
-      </c>
-      <c r="C24">
-        <v>1</v>
-      </c>
-      <c r="D24" t="s">
-        <v>10</v>
-      </c>
-      <c r="E24">
-        <v>1</v>
-      </c>
-      <c r="G24" t="s">
+      <c r="H24" t="s">
         <v>65</v>
-      </c>
-      <c r="H24" t="s">
-        <v>66</v>
       </c>
     </row>
     <row r="25" spans="1:5">
@@ -1706,53 +1703,53 @@
     </row>
     <row r="35" spans="1:1">
       <c r="A35" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="36" spans="1:1">
       <c r="A36" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="37" spans="1:1">
       <c r="A37" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="38" spans="1:1">
       <c r="A38" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="39" spans="1:1">
       <c r="A39" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="40" spans="1:1">
       <c r="A40" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="41" spans="1:1">
       <c r="A41" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="42" spans="1:1">
       <c r="A42" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="44" spans="1:5">
       <c r="A44" t="s">
-        <v>74</v>
-      </c>
-      <c r="B44" t="s">
-        <v>10</v>
-      </c>
-      <c r="C44" t="s">
-        <v>10</v>
+        <v>73</v>
+      </c>
+      <c r="B44">
+        <v>0</v>
+      </c>
+      <c r="C44">
+        <v>0</v>
       </c>
       <c r="D44">
         <v>4389</v>
@@ -1763,13 +1760,13 @@
     </row>
     <row r="45" spans="1:5">
       <c r="A45" t="s">
-        <v>75</v>
-      </c>
-      <c r="B45" t="s">
-        <v>10</v>
-      </c>
-      <c r="C45" t="s">
-        <v>10</v>
+        <v>74</v>
+      </c>
+      <c r="B45">
+        <v>0</v>
+      </c>
+      <c r="C45">
+        <v>0</v>
       </c>
       <c r="D45">
         <v>8</v>
@@ -1780,10 +1777,10 @@
     </row>
     <row r="46" spans="1:5">
       <c r="A46" t="s">
-        <v>76</v>
-      </c>
-      <c r="B46" t="s">
-        <v>10</v>
+        <v>75</v>
+      </c>
+      <c r="B46">
+        <v>0</v>
       </c>
       <c r="C46">
         <v>1</v>
@@ -1797,13 +1794,13 @@
     </row>
     <row r="48" spans="1:5">
       <c r="A48" t="s">
-        <v>77</v>
-      </c>
-      <c r="B48" t="s">
-        <v>10</v>
-      </c>
-      <c r="C48" t="s">
-        <v>10</v>
+        <v>76</v>
+      </c>
+      <c r="B48">
+        <v>0</v>
+      </c>
+      <c r="C48">
+        <v>0</v>
       </c>
       <c r="D48">
         <v>18</v>
@@ -1814,16 +1811,16 @@
     </row>
     <row r="49" spans="1:5">
       <c r="A49" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B49">
         <v>1</v>
       </c>
-      <c r="C49" t="s">
-        <v>10</v>
-      </c>
-      <c r="D49" t="s">
-        <v>10</v>
+      <c r="C49">
+        <v>0</v>
+      </c>
+      <c r="D49">
+        <v>0</v>
       </c>
       <c r="E49">
         <v>1</v>
@@ -1831,10 +1828,10 @@
     </row>
     <row r="51" spans="1:5">
       <c r="A51" t="s">
-        <v>79</v>
-      </c>
-      <c r="B51" t="s">
-        <v>10</v>
+        <v>78</v>
+      </c>
+      <c r="B51">
+        <v>0</v>
       </c>
       <c r="C51">
         <v>1</v>
@@ -1848,13 +1845,13 @@
     </row>
     <row r="52" spans="1:5">
       <c r="A52" t="s">
-        <v>80</v>
-      </c>
-      <c r="B52" t="s">
-        <v>10</v>
-      </c>
-      <c r="C52" t="s">
-        <v>10</v>
+        <v>79</v>
+      </c>
+      <c r="B52">
+        <v>0</v>
+      </c>
+      <c r="C52">
+        <v>0</v>
       </c>
       <c r="D52">
         <v>2</v>
@@ -1865,13 +1862,13 @@
     </row>
     <row r="53" spans="1:5">
       <c r="A53" t="s">
-        <v>81</v>
-      </c>
-      <c r="B53" t="s">
-        <v>10</v>
-      </c>
-      <c r="C53" t="s">
-        <v>10</v>
+        <v>80</v>
+      </c>
+      <c r="B53">
+        <v>0</v>
+      </c>
+      <c r="C53">
+        <v>0</v>
       </c>
       <c r="D53">
         <v>2</v>
@@ -1882,13 +1879,13 @@
     </row>
     <row r="55" spans="1:5">
       <c r="A55" t="s">
-        <v>82</v>
-      </c>
-      <c r="B55" t="s">
-        <v>10</v>
-      </c>
-      <c r="C55" t="s">
-        <v>10</v>
+        <v>81</v>
+      </c>
+      <c r="B55">
+        <v>0</v>
+      </c>
+      <c r="C55">
+        <v>0</v>
       </c>
       <c r="D55">
         <v>2</v>

</xml_diff>

<commit_message>
Correções nas querys, em um dado instanciado errado e resultados.
</commit_message>
<xml_diff>
--- a/dados/estabelecimentos/ago17.xlsx
+++ b/dados/estabelecimentos/ago17.xlsx
@@ -88,16 +88,16 @@
     <t>CntrSaude</t>
   </si>
   <si>
+    <t>CLINICA ESPECIALIZADA/AMBULATORIO ESPECIALIZADO</t>
+  </si>
+  <si>
+    <t>Clínica Especializada/ Ambulatório de Especialidades</t>
+  </si>
+  <si>
+    <t>ClincEspc</t>
+  </si>
+  <si>
     <t>UNIDADE MISTA</t>
-  </si>
-  <si>
-    <t>Clínica Especializada/ Ambulatório de Especialidades</t>
-  </si>
-  <si>
-    <t>ClincEspc</t>
-  </si>
-  <si>
-    <t>CLINICA ESPECIALIZADA/AMBULATORIO ESPECIALIZADO</t>
   </si>
   <si>
     <t>Consultório isolado</t>
@@ -268,9 +268,9 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
     <numFmt numFmtId="176" formatCode="_-&quot;R$&quot;* #,##0.00_-;\-&quot;R$&quot;* #,##0.00_-;_-&quot;R$&quot;* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="177" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="178" formatCode="_-&quot;R$&quot;* #,##0_-;\-&quot;R$&quot;* #,##0_-;_-&quot;R$&quot;* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="179" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="177" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="178" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="179" formatCode="_-&quot;R$&quot;* #,##0_-;\-&quot;R$&quot;* #,##0_-;_-&quot;R$&quot;* &quot;-&quot;_-;_-@_-"/>
   </numFmts>
   <fonts count="20">
     <font>
@@ -282,45 +282,14 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -342,10 +311,11 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color theme="3"/>
       <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -356,30 +326,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
+      <sz val="18"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -394,9 +342,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
+      <i/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -410,6 +358,35 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
@@ -418,8 +395,31 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -434,187 +434,187 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -625,17 +625,6 @@
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -663,6 +652,35 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FF7F7F7F"/>
       </left>
@@ -674,15 +692,6 @@
       </top>
       <bottom style="thin">
         <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -716,162 +725,153 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="13" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="20" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="16" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="27" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="27" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="10" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="14" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="14" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1200,8 +1200,8 @@
   <sheetPr/>
   <dimension ref="A1:H55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.2857142857143" defaultRowHeight="12.75" outlineLevelCol="7"/>
@@ -1367,16 +1367,16 @@
         <v>24</v>
       </c>
       <c r="B11">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C11">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D11">
-        <v>1</v>
+        <v>361</v>
       </c>
       <c r="E11">
-        <v>1</v>
+        <v>365</v>
       </c>
       <c r="G11" t="s">
         <v>25</v>
@@ -1390,16 +1390,16 @@
         <v>27</v>
       </c>
       <c r="B12">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C12">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D12">
-        <v>361</v>
+        <v>1</v>
       </c>
       <c r="E12">
-        <v>365</v>
+        <v>1</v>
       </c>
       <c r="G12" t="s">
         <v>28</v>

</xml_diff>